<commit_message>
dictionary support and parse setting support
</commit_message>
<xml_diff>
--- a/Kipon.Excel.UnitTests/Resources/ParsePropertySheetTest.xlsx
+++ b/Kipon.Excel.UnitTests/Resources/ParsePropertySheetTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\OpenSource\Kipon.Excel\Kipon.Excel.UnitTests\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41348047-2DB1-41B0-B706-5E97ECB5AEC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F427D4D9-E325-4A42-AA8D-EEA58F6E14E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="3720" windowWidth="28800" windowHeight="13575" xr2:uid="{B6489A87-1D11-48C5-A4F4-B8B6A8A5E741}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>first field</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>3c</t>
+  </si>
+  <si>
+    <t>P123661</t>
+  </si>
+  <si>
+    <t>P123662</t>
+  </si>
+  <si>
+    <t>P123663</t>
   </si>
 </sst>
 </file>
@@ -411,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D8BDFB8-DF81-4EEF-9DBF-E48D4CB6B7CD}">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -429,8 +438,17 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -440,8 +458,17 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>2</v>
       </c>
@@ -451,8 +478,17 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>3</v>
       </c>
@@ -461,6 +497,15 @@
       </c>
       <c r="D5" t="s">
         <v>8</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>60</v>
+      </c>
+      <c r="G5">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>